<commit_message>
Edited hernieuwde opdracht and globale planning, Added Use Cases
</commit_message>
<xml_diff>
--- a/KT1/KT1.1/KT1.1.2 Hernieuwde Opdracht/Moscow v1.0.0.xlsx
+++ b/KT1/KT1.1/KT1.1.2 Hernieuwde Opdracht/Moscow v1.0.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenley Strik\Documents\GitKraken\Periode_11_Proef_PVB_Tim_Kenley\Periode_11_Proef_PVB_Tim_Kenley\KT1\KT1.1\KT1.1.1 Hernieuwde Opdracht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenley Strik\Documents\GitKraken\Periode_11_Proef_PVB_Tim_Kenley\Periode_11_Proef_PVB_Tim_Kenley\KT1\KT1.1\KT1.1.2 Hernieuwde Opdracht\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Must have</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Hamburger menu</t>
+  </si>
+  <si>
+    <t>Simplistisch ontwerp</t>
+  </si>
+  <si>
+    <t>Huistijl van het bedrijf</t>
   </si>
 </sst>
 </file>
@@ -171,12 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -457,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +668,46 @@
       </c>
       <c r="E18" s="2"/>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Klassediagram and Datadictionary and some other changes
</commit_message>
<xml_diff>
--- a/KT1/KT1.1/KT1.1.2 Hernieuwde Opdracht/Moscow v1.0.0.xlsx
+++ b/KT1/KT1.1/KT1.1.2 Hernieuwde Opdracht/Moscow v1.0.0.xlsx
@@ -89,7 +89,7 @@
     <t>Simplistisch ontwerp</t>
   </si>
   <si>
-    <t>Huistijl van het bedrijf</t>
+    <t>Huisstijl van het bedrijf</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,8 +668,8 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -679,8 +679,8 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -690,8 +690,8 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="5"/>

</xml_diff>